<commit_message>
BAU: fix panderas failure cases index issue
..

..

..

..
</commit_message>
<xml_diff>
--- a/tests/integration_tests/mock_pf_returns/PF_Round_1_Validation_Failures.xlsx
+++ b/tests/integration_tests/mock_pf_returns/PF_Round_1_Validation_Failures.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PearceJ\stash\funding-service-design-post-award-data-store\tests\integration_tests\mock_pf_returns\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5424965B-D79C-4C37-844E-0905EB435357}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04566C8E-1410-4387-8DEF-768F6909F52B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="661" firstSheet="4" activeTab="10" xr2:uid="{F1A93CD4-AFD6-463B-B066-EB4D40A0C607}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="661" firstSheet="2" activeTab="2" xr2:uid="{F1A93CD4-AFD6-463B-B066-EB4D40A0C607}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="13" r:id="rId1"/>
@@ -115,7 +115,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2893" uniqueCount="1114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2892" uniqueCount="1113">
   <si>
     <t>Reporting Round</t>
   </si>
@@ -3743,9 +3743,6 @@
   </si>
   <si>
     <t>Head of Operations</t>
-  </si>
-  <si>
-    <t>einie</t>
   </si>
   <si>
     <t>inmv</t>
@@ -7897,8 +7894,8 @@
   </sheetPr>
   <dimension ref="A1:J177"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C179" sqref="C179"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8189,7 +8186,7 @@
         <v>299</v>
       </c>
       <c r="C48" s="125" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.35">
@@ -8311,7 +8308,7 @@
         <v>139</v>
       </c>
       <c r="C59" s="125" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.35">
@@ -8455,7 +8452,7 @@
         <v>331</v>
       </c>
       <c r="C72" s="125" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.35">
@@ -8466,7 +8463,7 @@
         <v>331</v>
       </c>
       <c r="C73" s="125" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.35">
@@ -8477,7 +8474,7 @@
         <v>331</v>
       </c>
       <c r="C74" s="125" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.35">
@@ -8488,7 +8485,7 @@
         <v>331</v>
       </c>
       <c r="C75" s="125" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.35">
@@ -8499,7 +8496,7 @@
         <v>331</v>
       </c>
       <c r="C76" s="125" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.35">
@@ -8510,7 +8507,7 @@
         <v>331</v>
       </c>
       <c r="C77" s="125" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.35">
@@ -8578,7 +8575,7 @@
         <v>342</v>
       </c>
       <c r="C84" s="125" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.35">
@@ -8589,7 +8586,7 @@
         <v>139</v>
       </c>
       <c r="C85" s="125" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.35">
@@ -8600,7 +8597,7 @@
         <v>139</v>
       </c>
       <c r="C86" s="125" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.35">
@@ -8721,7 +8718,7 @@
         <v>139</v>
       </c>
       <c r="C97" s="125" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.35">
@@ -8765,7 +8762,7 @@
         <v>342</v>
       </c>
       <c r="C101" s="125" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.35">
@@ -8798,7 +8795,7 @@
         <v>139</v>
       </c>
       <c r="C104" s="125" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.35">
@@ -16590,8 +16587,8 @@
   </sheetPr>
   <dimension ref="A1:P62"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -17072,8 +17069,8 @@
     </row>
     <row r="24" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="3"/>
-      <c r="B24" s="181" t="s">
-        <v>1110</v>
+      <c r="B24" s="181">
+        <v>0</v>
       </c>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
@@ -17176,7 +17173,9 @@
     </row>
     <row r="29" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="3"/>
-      <c r="B29" s="104"/>
+      <c r="B29" s="104">
+        <v>0</v>
+      </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
       <c r="E29" s="13"/>
@@ -17569,11 +17568,8 @@
       <formula1>$D$12:$D$27</formula1>
     </dataValidation>
   </dataValidations>
-  <hyperlinks>
-    <hyperlink ref="B24" r:id="rId1" display="test@testing.gov.uk" xr:uid="{47AF0A50-A9AD-46E2-80A8-D2E6DD22585B}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="landscape" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Calibri"&amp;10&amp;K000000 OFFICIAL - DLUHC USE ONLY&amp;1#_x000D_</oddHeader>
     <oddFooter>&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 OFFICIAL - DLUHC USE ONLY</oddFooter>
@@ -19841,7 +19837,7 @@
         <v>1</v>
       </c>
       <c r="G20" s="154" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
       <c r="H20" s="155">
         <v>4</v>
@@ -41981,7 +41977,7 @@
         <v>406</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="G9" s="80">
         <f>IFERROR(VALUE(LEFT(E9,1))*VALUE(LEFT(F9,1)),"N/A")</f>
@@ -42256,6 +42252,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="681fe441-c46c-4ea5-a5c5-b45872725697">
@@ -42275,7 +42280,7 @@
 </p:properties>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AB5DDB95A7ECBD49AA08D06BA3EF1CDA" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="fe5bfd8c052041f57bea8be2fc23aae3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="681fe441-c46c-4ea5-a5c5-b45872725697" xmlns:ns3="6bac55d2-c587-47e2-866b-bbb6fe14d104" xmlns:ns4="83a87e31-bf32-46ab-8e70-9fa18461fa4d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2f48421f1dce13a43278cc3c99628998" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -42546,16 +42551,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4FE8F99-283B-450B-9291-1D0662914CE9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{12714E09-E476-4024-A743-EBE78B46D4FD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -42568,7 +42572,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38A08E56-31DD-4856-904D-CF4B4BDF8261}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -42589,14 +42593,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4FE8F99-283B-450B-9291-1D0662914CE9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{95c71a0f-75e1-4c8f-90e2-641c9351dd98}" enabled="1" method="Standard" siteId="{3e0088dc-0629-4ae6-aa8c-813e7a296f50}" removed="0"/>

</xml_diff>